<commit_message>
New file containing just prompts and responses
</commit_message>
<xml_diff>
--- a/data/age/Age_ShortList_Categorized_Updated_Translated_Responses.xlsx
+++ b/data/age/Age_ShortList_Categorized_Updated_Translated_Responses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wesselb\dev\NoBBQ\data\age\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D13649F-08F6-4F02-ACA4-F383FB3493C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820D7630-3CB9-454D-B17E-D7CCAC15B504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53652" yWindow="-10980" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-11112" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -1183,19 +1183,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.36328125" customWidth="1"/>
+    <col min="1" max="1" width="22.36328125" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
     <col min="3" max="8" width="8.7265625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="91.453125" customWidth="1"/>
-    <col min="10" max="10" width="62.81640625" customWidth="1"/>
-    <col min="11" max="14" width="8.7265625" customWidth="1"/>
-    <col min="15" max="15" width="8.7265625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="52.08984375" customWidth="1"/>
+    <col min="10" max="10" width="19.08984375" customWidth="1"/>
+    <col min="11" max="14" width="8.7265625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="12.26953125" style="8" customWidth="1"/>
     <col min="16" max="16" width="8.7265625" style="8"/>
   </cols>
   <sheetData>

</xml_diff>